<commit_message>
dynamic source from text file
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>TECHNICAL EXAM</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Referral</t>
+  </si>
+  <si>
+    <t>Maureen Gwapa</t>
+  </si>
+  <si>
+    <t>Walk-in</t>
   </si>
 </sst>
 </file>
@@ -495,26 +501,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
     <col min="7" max="7" width="25.5703125" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" customWidth="1"/>
     <col min="9" max="9" width="21.5703125" customWidth="1"/>
     <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
     <col min="13" max="13" width="24" customWidth="1"/>
     <col min="14" max="14" width="21.5703125" customWidth="1"/>
   </cols>
@@ -614,6 +620,23 @@
         <v>124325434</v>
       </c>
     </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42915</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>5645645</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modified javascripts, partially added timer
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>TECHNICAL EXAM</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>JObstreet</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
   </si>
 </sst>
 </file>
@@ -510,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
@@ -697,6 +700,40 @@
         <v>943254</v>
       </c>
     </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42920</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>9233233212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>42920</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <v>9233233212</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
able to fetch results but in c#, modified some scripts..
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>TECHNICAL EXAM</t>
   </si>
@@ -61,45 +61,6 @@
   </si>
   <si>
     <t>Remarks</t>
-  </si>
-  <si>
-    <t>Kelly Marinduque</t>
-  </si>
-  <si>
-    <t>Hart Hart</t>
-  </si>
-  <si>
-    <t>Fiber Technician</t>
-  </si>
-  <si>
-    <t>Hart</t>
-  </si>
-  <si>
-    <t>System Administrator</t>
-  </si>
-  <si>
-    <t>Leah Mahusay</t>
-  </si>
-  <si>
-    <t>Referral</t>
-  </si>
-  <si>
-    <t>Maureen Gwapa</t>
-  </si>
-  <si>
-    <t>Walk-in</t>
-  </si>
-  <si>
-    <t>Naruto Uzumaki</t>
-  </si>
-  <si>
-    <t>HOIT Website</t>
-  </si>
-  <si>
-    <t>JObstreet</t>
-  </si>
-  <si>
-    <t>Harry Potter</t>
   </si>
 </sst>
 </file>
@@ -513,17 +474,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L2" sqref="A2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
@@ -582,157 +543,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>42914</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2">
-        <v>2454</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>42915</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3">
-        <v>565434</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>42915</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4">
-        <v>124325434</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>42915</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5">
-        <v>5645645</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>42915</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6">
-        <v>6534663</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>42915</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7">
-        <v>6534663</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>42916</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8">
-        <v>943254</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>42920</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9">
-        <v>9233233212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>42920</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10">
-        <v>9233233212</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added js timer but no sessions yet. added error checking for application form
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -63,10 +63,10 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Kelly Marinduque</t>
-  </si>
-  <si>
-    <t>LinkedIn</t>
+    <t>Sakura Haruno</t>
+  </si>
+  <si>
+    <t>HOIT Website</t>
   </si>
   <si>
     <t>Fiber Technician</t>
@@ -486,7 +486,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L2" sqref="A2:L2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +553,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42922</v>
+        <v>42923</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -565,7 +565,7 @@
         <v>16</v>
       </c>
       <c r="E2">
-        <v>9123435578</v>
+        <v>912343134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>